<commit_message>
Update: Cambios en formato de plantilla
</commit_message>
<xml_diff>
--- a/public/archivos/PlantillaParaErroresPadron.xlsx
+++ b/public/archivos/PlantillaParaErroresPadron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0226C59-0DCE-F14D-8F7D-B68175604E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19897AB-5E0F-9346-9303-778AC2D616EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4580" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Remesa</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Estatus Origen</t>
+  </si>
+  <si>
+    <t>EDAD</t>
   </si>
 </sst>
 </file>
@@ -639,6 +642,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -656,15 +668,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -981,215 +984,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A9C34E-97D7-7B4E-8969-873A36362A97}">
-  <dimension ref="A2:BS4"/>
+  <dimension ref="A2:BT4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="BK5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="AV5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BQ1" sqref="BQ1:BQ1048576"/>
+      <selection pane="bottomRight" activeCell="BB5" sqref="BB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="17.83203125" customWidth="1"/>
     <col min="55" max="55" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:71" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:71" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="BC3" s="18" t="s">
+    <row r="2" spans="1:72" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:72" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BC3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="BD3" s="19"/>
-      <c r="BE3" s="19"/>
-      <c r="BF3" s="19"/>
-      <c r="BG3" s="20" t="s">
+      <c r="BD3" s="22"/>
+      <c r="BE3" s="22"/>
+      <c r="BF3" s="22"/>
+      <c r="BG3" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="BH3" s="21"/>
-      <c r="BI3" s="22"/>
-      <c r="BJ3" s="20" t="s">
+      <c r="BH3" s="24"/>
+      <c r="BI3" s="25"/>
+      <c r="BJ3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="BK3" s="21"/>
-      <c r="BL3" s="21"/>
-      <c r="BM3" s="21"/>
-      <c r="BN3" s="22"/>
-      <c r="BO3" s="23"/>
+      <c r="BK3" s="24"/>
+      <c r="BL3" s="24"/>
+      <c r="BM3" s="24"/>
+      <c r="BN3" s="25"/>
+      <c r="BO3" s="26"/>
     </row>
-    <row r="4" spans="1:71" ht="78" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:72" ht="78" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AY4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="AZ4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AR4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AS4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AT4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AU4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AV4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AW4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AX4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AY4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AZ4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BA4" s="26" t="s">
+      <c r="BA4" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="BB4" s="26" t="s">
+      <c r="BB4" s="20" t="s">
         <v>42</v>
       </c>
       <c r="BC4" s="11" t="s">
@@ -1231,17 +1234,20 @@
       <c r="BO4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="BP4" s="25" t="s">
+      <c r="BP4" s="19" t="s">
         <v>57</v>
       </c>
       <c r="BQ4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="BR4" s="24" t="s">
+      <c r="BR4" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="BS4" s="17" t="s">
+      <c r="BS4" s="18" t="s">
         <v>62</v>
+      </c>
+      <c r="BT4" s="17" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: mostrar nombre rp cuando es diferente
</commit_message>
<xml_diff>
--- a/public/archivos/PlantillaParaErroresPadron.xlsx
+++ b/public/archivos/PlantillaParaErroresPadron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19897AB-5E0F-9346-9303-778AC2D616EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDA9F48-F35C-6649-95B2-58DB12715A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Remesa</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t>EDAD</t>
+  </si>
+  <si>
+    <t>NOMBRE RENAPO</t>
+  </si>
+  <si>
+    <t>APELLIDO 1 RENAPO</t>
+  </si>
+  <si>
+    <t>APELLIDO 2 RENAPO</t>
   </si>
 </sst>
 </file>
@@ -984,13 +993,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A9C34E-97D7-7B4E-8969-873A36362A97}">
-  <dimension ref="A2:BT4"/>
+  <dimension ref="A2:BW4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="AV5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="BI5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BB5" sqref="BB5"/>
+      <selection pane="bottomRight" activeCell="BL5" sqref="BL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,11 +1016,11 @@
     <col min="55" max="55" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="75" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:72" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:72" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="BC3" s="21" t="s">
         <v>43</v>
       </c>
@@ -1023,16 +1032,19 @@
       </c>
       <c r="BH3" s="24"/>
       <c r="BI3" s="25"/>
-      <c r="BJ3" s="23" t="s">
+      <c r="BJ3" s="25"/>
+      <c r="BK3" s="25"/>
+      <c r="BL3" s="25"/>
+      <c r="BM3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="BK3" s="24"/>
-      <c r="BL3" s="24"/>
-      <c r="BM3" s="24"/>
-      <c r="BN3" s="25"/>
-      <c r="BO3" s="26"/>
+      <c r="BN3" s="24"/>
+      <c r="BO3" s="24"/>
+      <c r="BP3" s="24"/>
+      <c r="BQ3" s="25"/>
+      <c r="BR3" s="26"/>
     </row>
-    <row r="4" spans="1:72" ht="78" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" ht="78" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1216,45 +1228,54 @@
       <c r="BI4" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="BJ4" s="13" t="s">
+      <c r="BJ4" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="BK4" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL4" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BM4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="BK4" s="14" t="s">
+      <c r="BN4" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="BL4" s="14" t="s">
+      <c r="BO4" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BM4" s="14" t="s">
+      <c r="BP4" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="BN4" s="15" t="s">
+      <c r="BQ4" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="BO4" s="15" t="s">
+      <c r="BR4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="BP4" s="19" t="s">
+      <c r="BS4" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="BQ4" s="16" t="s">
+      <c r="BT4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="BR4" s="18" t="s">
+      <c r="BU4" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="BS4" s="18" t="s">
+      <c r="BV4" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="BT4" s="17" t="s">
+      <c r="BW4" s="17" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="BC3:BF3"/>
-    <mergeCell ref="BG3:BI3"/>
-    <mergeCell ref="BJ3:BO3"/>
+    <mergeCell ref="BG3:BL3"/>
+    <mergeCell ref="BM3:BR3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add: Se agrega función para generar etiquetas en grupos vales y validación estatus origen
</commit_message>
<xml_diff>
--- a/public/archivos/PlantillaParaErroresPadron.xlsx
+++ b/public/archivos/PlantillaParaErroresPadron.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDA9F48-F35C-6649-95B2-58DB12715A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABF86CE-8CA6-044E-A18D-2016A9599E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Remesa</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>APELLIDO 2 RENAPO</t>
+  </si>
+  <si>
+    <t>ESTATUS ORIGEN</t>
+  </si>
+  <si>
+    <t>ESTATUS COMITÉ</t>
   </si>
 </sst>
 </file>
@@ -993,13 +999,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A9C34E-97D7-7B4E-8969-873A36362A97}">
-  <dimension ref="A2:BW4"/>
+  <dimension ref="A2:BY4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="BI5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="BT5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BL5" sqref="BL5"/>
+      <selection pane="bottomRight" activeCell="BX4" sqref="BX4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,11 +1022,12 @@
     <col min="55" max="55" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="75" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="29" customWidth="1"/>
+    <col min="76" max="77" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:75" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:75" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:77" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="BC3" s="21" t="s">
         <v>43</v>
       </c>
@@ -1044,7 +1051,7 @@
       <c r="BQ3" s="25"/>
       <c r="BR3" s="26"/>
     </row>
-    <row r="4" spans="1:75" ht="78" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" ht="78" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1267,8 +1274,14 @@
       <c r="BV4" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="BW4" s="17" t="s">
+      <c r="BW4" s="18" t="s">
         <v>73</v>
+      </c>
+      <c r="BX4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="BY4" s="17" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>